<commit_message>
Database updated with new footprints from EK
</commit_message>
<xml_diff>
--- a/Footprints/C655_Main_Board_Footprints_200210.xlsx
+++ b/Footprints/C655_Main_Board_Footprints_200210.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erlendm\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erlendm\OneDrive - Tomra\Arbeidsfiler\GitHub\Tomra_Altium_Library_GitHub\Footprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00FA851-567C-42B9-8CDF-AFA10DCA6149}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{E00FA851-567C-42B9-8CDF-AFA10DCA6149}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{55D19AC8-2A41-456B-8129-DD6658A6C869}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="595">
   <si>
     <t>Comment</t>
   </si>
@@ -1809,6 +1809,12 @@
   </si>
   <si>
     <t>silk too close to pad</t>
+  </si>
+  <si>
+    <t>added</t>
+  </si>
+  <si>
+    <t>Footprints\C655_Main_Board_EK.PcbLib</t>
   </si>
 </sst>
 </file>
@@ -2258,10 +2264,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I126"/>
+  <dimension ref="A1:J126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2270,6 +2276,7 @@
     <col min="3" max="3" width="25.85546875" customWidth="1"/>
     <col min="4" max="4" width="34.42578125" customWidth="1"/>
     <col min="5" max="6" width="17.7109375" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -2610,7 +2617,7 @@
       </c>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
@@ -2631,7 +2638,7 @@
       </c>
       <c r="G17" s="15"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>190</v>
       </c>
@@ -2651,8 +2658,11 @@
         <v>21</v>
       </c>
       <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>258</v>
       </c>
@@ -2673,7 +2683,7 @@
       </c>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>277</v>
       </c>
@@ -2694,7 +2704,7 @@
       </c>
       <c r="G20" s="7"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>57</v>
       </c>
@@ -2715,7 +2725,7 @@
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>47</v>
       </c>
@@ -2736,7 +2746,7 @@
       </c>
       <c r="G22" s="7"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>52</v>
       </c>
@@ -2757,7 +2767,7 @@
       </c>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>80</v>
       </c>
@@ -2778,7 +2788,7 @@
       </c>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>245</v>
       </c>
@@ -2803,8 +2813,11 @@
       <c r="H25" s="12" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" s="12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>107</v>
       </c>
@@ -2829,8 +2842,11 @@
       <c r="H26" s="12" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" s="12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>98</v>
       </c>
@@ -2851,7 +2867,7 @@
       </c>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>62</v>
       </c>
@@ -2872,7 +2888,7 @@
       </c>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>236</v>
       </c>
@@ -2893,7 +2909,7 @@
       </c>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>241</v>
       </c>
@@ -2918,8 +2934,11 @@
       <c r="H30" s="12" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30" s="12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>249</v>
       </c>
@@ -2944,8 +2963,11 @@
       <c r="H31" s="12" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31" s="12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>398</v>
       </c>
@@ -2966,7 +2988,7 @@
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>162</v>
       </c>
@@ -2987,7 +3009,7 @@
       </c>
       <c r="G33" s="7"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>349</v>
       </c>
@@ -3008,7 +3030,7 @@
       </c>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>129</v>
       </c>
@@ -3029,7 +3051,7 @@
       </c>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>93</v>
       </c>
@@ -3050,7 +3072,7 @@
       </c>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>25</v>
       </c>
@@ -3071,7 +3093,7 @@
       </c>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>103</v>
       </c>
@@ -3092,7 +3114,7 @@
       </c>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>11</v>
       </c>
@@ -3113,7 +3135,7 @@
       </c>
       <c r="G39" s="7"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
         <v>463</v>
       </c>
@@ -3139,10 +3161,13 @@
         <v>591</v>
       </c>
       <c r="I40" s="12" t="s">
+        <v>593</v>
+      </c>
+      <c r="J40" s="12" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>475</v>
       </c>
@@ -3163,7 +3188,7 @@
       </c>
       <c r="G41" s="7"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>441</v>
       </c>
@@ -3184,7 +3209,7 @@
       </c>
       <c r="G42" s="7"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>364</v>
       </c>
@@ -3205,7 +3230,7 @@
       </c>
       <c r="G43" s="7"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>369</v>
       </c>
@@ -3226,7 +3251,7 @@
       </c>
       <c r="G44" s="7"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>484</v>
       </c>
@@ -3247,7 +3272,7 @@
       </c>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
         <v>394</v>
       </c>
@@ -3272,8 +3297,11 @@
       <c r="H46" s="12" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I46" s="12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>20</v>
       </c>
@@ -3294,7 +3322,7 @@
       </c>
       <c r="G47" s="7"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>499</v>
       </c>
@@ -3315,7 +3343,7 @@
       </c>
       <c r="G48" s="7"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
         <v>451</v>
       </c>
@@ -3340,8 +3368,11 @@
       <c r="H49" s="12" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I49" s="12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>513</v>
       </c>
@@ -3365,7 +3396,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>157</v>
       </c>
@@ -3389,7 +3420,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>75</v>
       </c>
@@ -3410,7 +3441,7 @@
       </c>
       <c r="G52" s="7"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>6</v>
       </c>
@@ -3431,7 +3462,7 @@
       </c>
       <c r="G53" s="7"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>16</v>
       </c>
@@ -3452,7 +3483,7 @@
       </c>
       <c r="G54" s="7"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>30</v>
       </c>
@@ -3473,7 +3504,7 @@
       </c>
       <c r="G55" s="7"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>34</v>
       </c>
@@ -3494,7 +3525,7 @@
       </c>
       <c r="G56" s="7"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>38</v>
       </c>
@@ -3515,7 +3546,7 @@
       </c>
       <c r="G57" s="7"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>67</v>
       </c>
@@ -3536,7 +3567,7 @@
       </c>
       <c r="G58" s="7"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>71</v>
       </c>
@@ -3557,7 +3588,7 @@
       </c>
       <c r="G59" s="7"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>85</v>
       </c>
@@ -3578,7 +3609,7 @@
       </c>
       <c r="G60" s="7"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>89</v>
       </c>
@@ -3599,7 +3630,7 @@
       </c>
       <c r="G61" s="7"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
         <v>268</v>
       </c>
@@ -3624,8 +3655,11 @@
       <c r="H62" s="12" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I62" s="12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>374</v>
       </c>
@@ -3646,7 +3680,7 @@
       </c>
       <c r="G63" s="7"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>504</v>
       </c>
@@ -3667,7 +3701,7 @@
       </c>
       <c r="G64" s="7"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>359</v>
       </c>
@@ -3688,7 +3722,7 @@
       </c>
       <c r="G65" s="7"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>176</v>
       </c>
@@ -3709,7 +3743,7 @@
       </c>
       <c r="G66" s="7"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>522</v>
       </c>
@@ -3733,7 +3767,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
         <v>467</v>
       </c>
@@ -3758,8 +3792,11 @@
       <c r="H68" s="12" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I68" s="12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>556</v>
       </c>
@@ -3780,7 +3817,7 @@
       </c>
       <c r="G69" s="7"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>42</v>
       </c>
@@ -3801,7 +3838,7 @@
       </c>
       <c r="G70" s="7"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
         <v>455</v>
       </c>
@@ -3826,8 +3863,11 @@
       <c r="H71" s="12" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I71" s="12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="8" t="s">
         <v>422</v>
       </c>
@@ -3852,8 +3892,11 @@
       <c r="H72" s="12" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I72" s="12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>459</v>
       </c>
@@ -3877,7 +3920,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>417</v>
       </c>
@@ -3898,7 +3941,7 @@
       </c>
       <c r="G74" s="7"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>407</v>
       </c>
@@ -3919,7 +3962,7 @@
       </c>
       <c r="G75" s="7"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>431</v>
       </c>
@@ -3940,7 +3983,7 @@
       </c>
       <c r="G76" s="7"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>530</v>
       </c>
@@ -3961,7 +4004,7 @@
       </c>
       <c r="G77" s="7"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="8" t="s">
         <v>535</v>
       </c>
@@ -3986,8 +4029,11 @@
       <c r="H78" s="12" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I78" s="12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>446</v>
       </c>
@@ -4008,7 +4054,7 @@
       </c>
       <c r="G79" s="7"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>471</v>
       </c>
@@ -4365,7 +4411,7 @@
       </c>
       <c r="G96" s="7"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="8" t="s">
         <v>552</v>
       </c>
@@ -4390,8 +4436,11 @@
       <c r="H97" s="12" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I97" s="12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>185</v>
       </c>
@@ -4412,7 +4461,7 @@
       </c>
       <c r="G98" s="7"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>344</v>
       </c>
@@ -4433,7 +4482,7 @@
       </c>
       <c r="G99" s="7"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>436</v>
       </c>
@@ -4454,7 +4503,7 @@
       </c>
       <c r="G100" s="7"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>231</v>
       </c>
@@ -4475,7 +4524,7 @@
       </c>
       <c r="G101" s="7"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>317</v>
       </c>
@@ -4499,7 +4548,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>320</v>
       </c>
@@ -4520,7 +4569,7 @@
       </c>
       <c r="G103" s="7"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>354</v>
       </c>
@@ -4541,7 +4590,7 @@
       </c>
       <c r="G104" s="7"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>208</v>
       </c>
@@ -4562,7 +4611,7 @@
       </c>
       <c r="G105" s="7"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>138</v>
       </c>
@@ -4583,7 +4632,7 @@
       </c>
       <c r="G106" s="7"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>217</v>
       </c>
@@ -4607,7 +4656,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="8" t="s">
         <v>213</v>
       </c>
@@ -4632,8 +4681,11 @@
       <c r="H108" s="12" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I108" s="12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>412</v>
       </c>
@@ -4654,7 +4706,7 @@
       </c>
       <c r="G109" s="7"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>263</v>
       </c>
@@ -4675,7 +4727,7 @@
       </c>
       <c r="G110" s="7"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>263</v>
       </c>
@@ -4696,7 +4748,7 @@
       </c>
       <c r="G111" s="7"/>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>384</v>
       </c>

</xml_diff>

<commit_message>
Fixed broken footprint reference for 17074106
</commit_message>
<xml_diff>
--- a/Footprints/C655_Main_Board_Footprints_200210.xlsx
+++ b/Footprints/C655_Main_Board_Footprints_200210.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erlendm\OneDrive - Tomra\Arbeidsfiler\GitHub\Tomra_Altium_Library_GitHub\Footprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{E00FA851-567C-42B9-8CDF-AFA10DCA6149}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{55D19AC8-2A41-456B-8129-DD6658A6C869}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{E00FA851-567C-42B9-8CDF-AFA10DCA6149}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5EA57834-1900-4DF0-9853-02A664303135}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2267,7 +2267,7 @@
   <dimension ref="A1:J126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+      <selection activeCell="E16" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2279,7 +2279,7 @@
     <col min="10" max="10" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>325</v>
       </c>
@@ -2302,520 +2302,515 @@
         <v>578</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>193</v>
+        <v>311</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>194</v>
+        <v>312</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>197</v>
+        <v>576</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="E2" s="5">
+        <v>61413002</v>
       </c>
       <c r="F2" s="6">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>221</v>
+        <v>311</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>222</v>
+        <v>312</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>225</v>
+        <v>577</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="E3" s="5">
+        <v>61413003</v>
       </c>
       <c r="F3" s="6">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>226</v>
+        <v>349</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>227</v>
+        <v>350</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>228</v>
+        <v>351</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>229</v>
+        <v>352</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>230</v>
+        <v>353</v>
       </c>
       <c r="F4" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>286</v>
+        <v>354</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>287</v>
+        <v>355</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>288</v>
+        <v>356</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>289</v>
+        <v>357</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>290</v>
+        <v>358</v>
       </c>
       <c r="F5" s="6">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>561</v>
+        <v>129</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>562</v>
+        <v>130</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>563</v>
+        <v>131</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>564</v>
+        <v>132</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>565</v>
+        <v>133</v>
       </c>
       <c r="F6" s="6">
         <v>1</v>
       </c>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>566</v>
+        <v>162</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>567</v>
+        <v>163</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>568</v>
+        <v>164</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>564</v>
+        <v>165</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>569</v>
+        <v>166</v>
       </c>
       <c r="F7" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>198</v>
+        <v>138</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>199</v>
+        <v>139</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>200</v>
+        <v>140</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>202</v>
+        <v>142</v>
       </c>
       <c r="F8" s="6">
         <v>1</v>
       </c>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>306</v>
+        <v>384</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>307</v>
+        <v>385</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>308</v>
+        <v>386</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>309</v>
+        <v>387</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>310</v>
+        <v>388</v>
       </c>
       <c r="F9" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>291</v>
+        <v>176</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>292</v>
+        <v>177</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>293</v>
+        <v>178</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>294</v>
+        <v>179</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>295</v>
+        <v>180</v>
       </c>
       <c r="F10" s="6">
+        <v>1</v>
+      </c>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="6">
         <v>3</v>
       </c>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="F11" s="6">
-        <v>2</v>
-      </c>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>296</v>
+        <v>52</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>297</v>
+        <v>53</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>298</v>
+        <v>54</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>299</v>
+        <v>55</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>300</v>
+        <v>56</v>
       </c>
       <c r="F12" s="6">
         <v>2</v>
       </c>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>148</v>
+        <v>80</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>149</v>
+        <v>81</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>150</v>
+        <v>82</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>151</v>
+        <v>83</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>152</v>
+        <v>84</v>
       </c>
       <c r="F13" s="6">
+        <v>3</v>
+      </c>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="6">
+        <v>3</v>
+      </c>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1</v>
+      </c>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="6">
+        <v>2</v>
+      </c>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="6">
         <v>6</v>
       </c>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F14" s="6">
-        <v>12</v>
-      </c>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="F15" s="6">
-        <v>2</v>
-      </c>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="F16" s="6">
-        <v>34</v>
-      </c>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" s="15"/>
+      <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>190</v>
+        <v>75</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>190</v>
+        <v>76</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>191</v>
+        <v>77</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>190</v>
+        <v>78</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>192</v>
+        <v>79</v>
       </c>
       <c r="F18" s="6">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="I18" t="s">
-        <v>594</v>
-      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>258</v>
+        <v>30</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>259</v>
+        <v>31</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>260</v>
+        <v>32</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>261</v>
+        <v>9</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>262</v>
+        <v>33</v>
       </c>
       <c r="F19" s="6">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>277</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>278</v>
+        <v>17</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>279</v>
+        <v>18</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>280</v>
+        <v>9</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>281</v>
+        <v>19</v>
       </c>
       <c r="F20" s="6">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="F21" s="6">
-        <v>3</v>
+        <v>189</v>
       </c>
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="F22" s="6">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="F23" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F24" s="6">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>246</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>582</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="F25" s="10">
-        <v>1</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>578</v>
-      </c>
-      <c r="H25" s="12" t="s">
-        <v>591</v>
-      </c>
-      <c r="I25" s="12" t="s">
-        <v>593</v>
-      </c>
+      <c r="A25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" s="6">
+        <v>21</v>
+      </c>
+      <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
@@ -2848,61 +2843,61 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>98</v>
+        <v>20</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>101</v>
+        <v>23</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="F27" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="F28" s="6">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>236</v>
+        <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>237</v>
+        <v>26</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>238</v>
+        <v>27</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>239</v>
+        <v>28</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>240</v>
+        <v>29</v>
       </c>
       <c r="F29" s="6">
         <v>2</v>
@@ -2910,1059 +2905,1010 @@
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>581</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="F30" s="10">
-        <v>2</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>578</v>
-      </c>
-      <c r="H30" s="12" t="s">
-        <v>591</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>593</v>
-      </c>
+      <c r="A30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="6">
+        <v>3</v>
+      </c>
+      <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>583</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="F31" s="10">
-        <v>2</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>578</v>
-      </c>
-      <c r="H31" s="12" t="s">
-        <v>591</v>
-      </c>
-      <c r="I31" s="12" t="s">
-        <v>593</v>
-      </c>
+      <c r="A31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" s="6">
+        <v>1</v>
+      </c>
+      <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>398</v>
+        <v>89</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>399</v>
+        <v>90</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>400</v>
+        <v>91</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>401</v>
+        <v>9</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>402</v>
+        <v>92</v>
       </c>
       <c r="F32" s="6">
+        <v>5</v>
+      </c>
+      <c r="G32" s="7"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F33" s="6">
         <v>1</v>
       </c>
-      <c r="G32" s="7"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="F33" s="6">
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F34" s="6">
+        <v>6</v>
+      </c>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="F35" s="6">
+        <v>363</v>
+      </c>
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="F36" s="6">
+        <v>106</v>
+      </c>
+      <c r="G36" s="7"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="F37" s="10">
+        <v>3</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>578</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>591</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F38" s="6">
+        <v>7</v>
+      </c>
+      <c r="G38" s="7"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="F39" s="6">
         <v>2</v>
       </c>
-      <c r="G33" s="7"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="F34" s="6">
-        <v>4</v>
-      </c>
-      <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="F35" s="6">
+      <c r="G39" s="7"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="F40" s="6">
         <v>1</v>
       </c>
-      <c r="G35" s="7"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F36" s="6">
+      <c r="G40" s="7"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="F41" s="10">
         <v>1</v>
       </c>
-      <c r="G36" s="7"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F37" s="6">
-        <v>2</v>
-      </c>
-      <c r="G37" s="7"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="F38" s="6">
-        <v>1</v>
-      </c>
-      <c r="G38" s="7"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F39" s="6">
-        <v>3</v>
-      </c>
-      <c r="G39" s="7"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="8" t="s">
-        <v>463</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>464</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>465</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>478</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>466</v>
-      </c>
-      <c r="F40" s="10">
-        <v>10</v>
-      </c>
-      <c r="G40" s="11" t="s">
+      <c r="G41" s="11" t="s">
         <v>578</v>
       </c>
-      <c r="H40" s="12" t="s">
+      <c r="H41" s="12" t="s">
         <v>591</v>
       </c>
-      <c r="I40" s="12" t="s">
+      <c r="I41" s="12" t="s">
         <v>593</v>
       </c>
-      <c r="J40" s="12" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>479</v>
-      </c>
-      <c r="F41" s="6">
-        <v>2</v>
-      </c>
-      <c r="G41" s="7"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>441</v>
+        <v>253</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>442</v>
+        <v>254</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>443</v>
+        <v>255</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>444</v>
+        <v>256</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>445</v>
+        <v>257</v>
       </c>
       <c r="F42" s="6">
         <v>1</v>
       </c>
       <c r="G42" s="7"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="F43" s="6">
+        <v>1</v>
+      </c>
+      <c r="G43" s="7"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="F44" s="6">
+        <v>4</v>
+      </c>
+      <c r="G44" s="7"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="F45" s="6">
+        <v>2</v>
+      </c>
+      <c r="G45" s="7"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="F46" s="6">
+        <v>1</v>
+      </c>
+      <c r="G46" s="7"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F47" s="6">
+        <v>17</v>
+      </c>
+      <c r="G47" s="7"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F48" s="6">
+        <v>16</v>
+      </c>
+      <c r="G48" s="7"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F49" s="6">
+        <v>35</v>
+      </c>
+      <c r="G49" s="7"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F50" s="6">
+        <v>2</v>
+      </c>
+      <c r="G50" s="7"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F51" s="6">
+        <v>34</v>
+      </c>
+      <c r="G51" s="7"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F52" s="6">
+        <v>3</v>
+      </c>
+      <c r="G52" s="7"/>
+      <c r="H52" s="17" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F53" s="6">
+        <v>2</v>
+      </c>
+      <c r="G53" s="7"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F54" s="6">
+        <v>5</v>
+      </c>
+      <c r="G54" s="7"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F55" s="6">
+        <v>6</v>
+      </c>
+      <c r="G55" s="7"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F56" s="6">
+        <v>12</v>
+      </c>
+      <c r="G56" s="7"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="F57" s="6">
+        <v>10</v>
+      </c>
+      <c r="G57" s="7"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="F58" s="6">
+        <v>1</v>
+      </c>
+      <c r="G58" s="7"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="F59" s="6">
+        <v>2</v>
+      </c>
+      <c r="G59" s="7"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="F60" s="6">
+        <v>8</v>
+      </c>
+      <c r="G60" s="7"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="F61" s="6">
+        <v>2</v>
+      </c>
+      <c r="G61" s="7"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="F62" s="6">
+        <v>3</v>
+      </c>
+      <c r="G62" s="7"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D63" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E63" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="F43" s="6">
+      <c r="F63" s="6">
         <v>2</v>
       </c>
-      <c r="G43" s="7"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="F44" s="6">
-        <v>1</v>
-      </c>
-      <c r="G44" s="7"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>488</v>
-      </c>
-      <c r="F45" s="6">
-        <v>1</v>
-      </c>
-      <c r="G45" s="7"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" s="8" t="s">
-        <v>394</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>589</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>397</v>
-      </c>
-      <c r="F46" s="10">
-        <v>3</v>
-      </c>
-      <c r="G46" s="11" t="s">
-        <v>578</v>
-      </c>
-      <c r="H46" s="12" t="s">
-        <v>591</v>
-      </c>
-      <c r="I46" s="12" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F47" s="6">
-        <v>1</v>
-      </c>
-      <c r="G47" s="7"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>503</v>
-      </c>
-      <c r="F48" s="6">
-        <v>6</v>
-      </c>
-      <c r="G48" s="7"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
-        <v>451</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>452</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>453</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>586</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>454</v>
-      </c>
-      <c r="F49" s="10">
-        <v>1</v>
-      </c>
-      <c r="G49" s="11" t="s">
-        <v>578</v>
-      </c>
-      <c r="H49" s="12" t="s">
-        <v>591</v>
-      </c>
-      <c r="I49" s="12" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>516</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>517</v>
-      </c>
-      <c r="F50" s="6">
-        <v>4</v>
-      </c>
-      <c r="G50" s="7"/>
-      <c r="H50" s="17" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>570</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="F51" s="6">
-        <v>3</v>
-      </c>
-      <c r="G51" s="7"/>
-      <c r="H51" s="17" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F52" s="6">
-        <v>13</v>
-      </c>
-      <c r="G52" s="7"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F53" s="6">
-        <v>189</v>
-      </c>
-      <c r="G53" s="7"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F54" s="6">
-        <v>16</v>
-      </c>
-      <c r="G54" s="7"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F55" s="6">
-        <v>38</v>
-      </c>
-      <c r="G55" s="7"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F56" s="6">
-        <v>1</v>
-      </c>
-      <c r="G56" s="7"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F57" s="6">
-        <v>12</v>
-      </c>
-      <c r="G57" s="7"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F58" s="6">
-        <v>21</v>
-      </c>
-      <c r="G58" s="7"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F59" s="6">
-        <v>12</v>
-      </c>
-      <c r="G59" s="7"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F60" s="6">
-        <v>4</v>
-      </c>
-      <c r="G60" s="7"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F61" s="6">
-        <v>5</v>
-      </c>
-      <c r="G61" s="7"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>584</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="F62" s="10">
-        <v>1</v>
-      </c>
-      <c r="G62" s="11" t="s">
-        <v>578</v>
-      </c>
-      <c r="H62" s="12" t="s">
-        <v>591</v>
-      </c>
-      <c r="I62" s="12" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="F63" s="6">
+      <c r="G63" s="7"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E64" s="5" t="s">
         <v>363</v>
       </c>
-      <c r="G63" s="7"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>506</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>508</v>
-      </c>
       <c r="F64" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G64" s="7"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>359</v>
+        <v>296</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>360</v>
+        <v>297</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>361</v>
+        <v>298</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>362</v>
+        <v>299</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>363</v>
+        <v>300</v>
       </c>
       <c r="F65" s="6">
         <v>2</v>
       </c>
       <c r="G65" s="7"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>176</v>
+        <v>291</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>177</v>
+        <v>292</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>178</v>
+        <v>293</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>179</v>
+        <v>294</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>180</v>
+        <v>295</v>
       </c>
       <c r="F66" s="6">
+        <v>3</v>
+      </c>
+      <c r="G66" s="7"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="F67" s="6">
+        <v>2</v>
+      </c>
+      <c r="G67" s="7"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="F68" s="6">
+        <v>2</v>
+      </c>
+      <c r="G68" s="7"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="F69" s="6">
+        <v>2</v>
+      </c>
+      <c r="G69" s="7"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>517</v>
+      </c>
+      <c r="F70" s="6">
+        <v>4</v>
+      </c>
+      <c r="G70" s="7"/>
+      <c r="H70" s="17" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="F71" s="6">
         <v>1</v>
       </c>
-      <c r="G66" s="7"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>572</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>525</v>
-      </c>
-      <c r="F67" s="6">
+      <c r="G71" s="7"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="F72" s="6">
         <v>1</v>
       </c>
-      <c r="G67" s="7"/>
-      <c r="H67" s="17" t="s">
+      <c r="G72" s="7"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="F73" s="6">
+        <v>1</v>
+      </c>
+      <c r="G73" s="7"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>452</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="F74" s="10">
+        <v>1</v>
+      </c>
+      <c r="G74" s="11" t="s">
+        <v>578</v>
+      </c>
+      <c r="H74" s="12" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A68" s="8" t="s">
+      <c r="I74" s="12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" s="8" t="s">
         <v>467</v>
       </c>
-      <c r="B68" s="8" t="s">
+      <c r="B75" s="8" t="s">
         <v>468</v>
       </c>
-      <c r="C68" s="8" t="s">
+      <c r="C75" s="8" t="s">
         <v>469</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D75" s="3" t="s">
         <v>559</v>
       </c>
-      <c r="E68" s="9" t="s">
+      <c r="E75" s="9" t="s">
         <v>470</v>
       </c>
-      <c r="F68" s="10">
+      <c r="F75" s="10">
         <v>1</v>
       </c>
-      <c r="G68" s="11" t="s">
+      <c r="G75" s="11" t="s">
         <v>578</v>
       </c>
-      <c r="H68" s="12" t="s">
+      <c r="H75" s="12" t="s">
         <v>591</v>
       </c>
-      <c r="I68" s="12" t="s">
+      <c r="I75" s="12" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
-        <v>556</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>557</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>558</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>560</v>
-      </c>
-      <c r="F69" s="6">
-        <v>1</v>
-      </c>
-      <c r="G69" s="7"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F70" s="6">
-        <v>9</v>
-      </c>
-      <c r="G70" s="7"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A71" s="8" t="s">
-        <v>455</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>456</v>
-      </c>
-      <c r="C71" s="8" t="s">
-        <v>457</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>587</v>
-      </c>
-      <c r="E71" s="9" t="s">
-        <v>458</v>
-      </c>
-      <c r="F71" s="10">
-        <v>3</v>
-      </c>
-      <c r="G71" s="11" t="s">
-        <v>578</v>
-      </c>
-      <c r="H71" s="12" t="s">
-        <v>591</v>
-      </c>
-      <c r="I71" s="12" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A72" s="8" t="s">
-        <v>422</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>423</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>424</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>585</v>
-      </c>
-      <c r="E72" s="9" t="s">
-        <v>425</v>
-      </c>
-      <c r="F72" s="10">
-        <v>1</v>
-      </c>
-      <c r="G72" s="11" t="s">
-        <v>578</v>
-      </c>
-      <c r="H72" s="12" t="s">
-        <v>591</v>
-      </c>
-      <c r="I72" s="12" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>590</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>462</v>
-      </c>
-      <c r="F73" s="6">
-        <v>6</v>
-      </c>
-      <c r="G73" s="7"/>
-      <c r="H73" s="17" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>421</v>
-      </c>
-      <c r="F74" s="6">
-        <v>1</v>
-      </c>
-      <c r="G74" s="7"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="F75" s="6">
-        <v>2</v>
-      </c>
-      <c r="G75" s="7"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>431</v>
       </c>
@@ -3983,586 +3929,624 @@
       </c>
       <c r="G76" s="7"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>531</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>534</v>
-      </c>
-      <c r="F77" s="6">
-        <v>2</v>
-      </c>
-      <c r="G77" s="7"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A78" s="8" t="s">
-        <v>535</v>
-      </c>
-      <c r="B78" s="8" t="s">
-        <v>536</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>537</v>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>464</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>466</v>
+      </c>
+      <c r="F77" s="10">
+        <v>10</v>
+      </c>
+      <c r="G77" s="11" t="s">
+        <v>578</v>
+      </c>
+      <c r="H77" s="12" t="s">
+        <v>591</v>
+      </c>
+      <c r="I77" s="12" t="s">
+        <v>593</v>
+      </c>
+      <c r="J77" s="12" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>461</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="E78" s="9" t="s">
-        <v>538</v>
-      </c>
-      <c r="F78" s="10">
-        <v>1</v>
-      </c>
-      <c r="G78" s="11" t="s">
-        <v>578</v>
-      </c>
-      <c r="H78" s="12" t="s">
+        <v>590</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="F78" s="6">
+        <v>6</v>
+      </c>
+      <c r="G78" s="7"/>
+      <c r="H78" s="17" t="s">
         <v>591</v>
       </c>
-      <c r="I78" s="12" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>446</v>
+        <v>494</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>447</v>
+        <v>495</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>448</v>
+        <v>496</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>449</v>
+        <v>497</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>450</v>
+        <v>498</v>
       </c>
       <c r="F79" s="6">
         <v>2</v>
       </c>
       <c r="G79" s="7"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>471</v>
+        <v>417</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>472</v>
+        <v>418</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>473</v>
+        <v>419</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>449</v>
+        <v>420</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>474</v>
+        <v>421</v>
       </c>
       <c r="F80" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G80" s="7"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="E81" s="5" t="s">
-        <v>483</v>
-      </c>
-      <c r="F81" s="6">
-        <v>2</v>
-      </c>
-      <c r="G81" s="7"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" s="8" t="s">
+        <v>422</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>423</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="F81" s="10">
+        <v>1</v>
+      </c>
+      <c r="G81" s="11" t="s">
+        <v>578</v>
+      </c>
+      <c r="H81" s="12" t="s">
+        <v>591</v>
+      </c>
+      <c r="I81" s="12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>526</v>
+        <v>484</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>527</v>
+        <v>485</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>528</v>
+        <v>486</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>449</v>
+        <v>487</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>529</v>
+        <v>488</v>
       </c>
       <c r="F82" s="6">
         <v>1</v>
       </c>
       <c r="G82" s="7"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>489</v>
+        <v>556</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>490</v>
+        <v>557</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>491</v>
+        <v>558</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>492</v>
+        <v>559</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>493</v>
+        <v>560</v>
       </c>
       <c r="F83" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G83" s="7"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>509</v>
+        <v>526</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>510</v>
+        <v>527</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>511</v>
+        <v>528</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>492</v>
+        <v>449</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>512</v>
+        <v>529</v>
       </c>
       <c r="F84" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G84" s="7"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>120</v>
+        <v>518</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>121</v>
+        <v>519</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>122</v>
+        <v>520</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>123</v>
+        <v>429</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>124</v>
+        <v>521</v>
       </c>
       <c r="F85" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G85" s="7"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>125</v>
+        <v>548</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>126</v>
+        <v>549</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>127</v>
+        <v>550</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>123</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>128</v>
+        <v>551</v>
       </c>
       <c r="F86" s="6">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="G86" s="7"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="F87" s="6">
-        <v>16</v>
-      </c>
-      <c r="G87" s="7"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" s="8" t="s">
+        <v>552</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>553</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>554</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>555</v>
+      </c>
+      <c r="F87" s="10">
+        <v>1</v>
+      </c>
+      <c r="G87" s="11" t="s">
+        <v>578</v>
+      </c>
+      <c r="H87" s="12" t="s">
+        <v>591</v>
+      </c>
+      <c r="I87" s="12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>328</v>
+        <v>426</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>329</v>
+        <v>427</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>330</v>
+        <v>428</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>123</v>
+        <v>429</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>331</v>
+        <v>430</v>
       </c>
       <c r="F88" s="6">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G88" s="7"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="F89" s="6">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" s="8" t="s">
+        <v>535</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>536</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>537</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>538</v>
+      </c>
+      <c r="F89" s="10">
+        <v>1</v>
+      </c>
+      <c r="G89" s="11" t="s">
+        <v>578</v>
+      </c>
+      <c r="H89" s="12" t="s">
+        <v>591</v>
+      </c>
+      <c r="I89" s="12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="F90" s="6">
+        <v>2</v>
+      </c>
+      <c r="G90" s="7"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" s="8" t="s">
+        <v>455</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>457</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="E91" s="9" t="s">
+        <v>458</v>
+      </c>
+      <c r="F91" s="10">
         <v>3</v>
       </c>
-      <c r="G89" s="7"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E90" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="F90" s="6">
-        <v>8</v>
-      </c>
-      <c r="G90" s="7"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E91" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="F91" s="6">
-        <v>2</v>
-      </c>
-      <c r="G91" s="7"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G91" s="11" t="s">
+        <v>578</v>
+      </c>
+      <c r="H91" s="12" t="s">
+        <v>591</v>
+      </c>
+      <c r="I91" s="12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>548</v>
+        <v>471</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>549</v>
+        <v>472</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>550</v>
+        <v>473</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>123</v>
+        <v>449</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>551</v>
+        <v>474</v>
       </c>
       <c r="F92" s="6">
         <v>2</v>
       </c>
       <c r="G92" s="7"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>426</v>
+        <v>499</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>427</v>
+        <v>500</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>428</v>
+        <v>501</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>429</v>
+        <v>502</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>430</v>
+        <v>503</v>
       </c>
       <c r="F93" s="6">
+        <v>6</v>
+      </c>
+      <c r="G93" s="7"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="F94" s="6">
+        <v>2</v>
+      </c>
+      <c r="G94" s="7"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="F95" s="6">
+        <v>5</v>
+      </c>
+      <c r="G95" s="7"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="F96" s="6">
+        <v>2</v>
+      </c>
+      <c r="G96" s="7"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>543</v>
+      </c>
+      <c r="F97" s="6">
         <v>1</v>
       </c>
-      <c r="G93" s="7"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A94" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="E94" s="5" t="s">
-        <v>521</v>
-      </c>
-      <c r="F94" s="6">
-        <v>1</v>
-      </c>
-      <c r="G94" s="7"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A95" s="1" t="s">
-        <v>539</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>540</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>541</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="E95" s="5" t="s">
-        <v>543</v>
-      </c>
-      <c r="F95" s="6">
-        <v>1</v>
-      </c>
-      <c r="G95" s="7"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A96" s="1" t="s">
-        <v>544</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="E96" s="5" t="s">
-        <v>547</v>
-      </c>
-      <c r="F96" s="6">
-        <v>1</v>
-      </c>
-      <c r="G96" s="7"/>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A97" s="8" t="s">
-        <v>552</v>
-      </c>
-      <c r="B97" s="8" t="s">
-        <v>553</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>554</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>588</v>
-      </c>
-      <c r="E97" s="9" t="s">
-        <v>555</v>
-      </c>
-      <c r="F97" s="10">
-        <v>1</v>
-      </c>
-      <c r="G97" s="11" t="s">
-        <v>578</v>
-      </c>
-      <c r="H97" s="12" t="s">
-        <v>591</v>
-      </c>
-      <c r="I97" s="12" t="s">
-        <v>593</v>
-      </c>
+      <c r="G97" s="7"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>185</v>
+        <v>544</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>186</v>
+        <v>545</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>187</v>
+        <v>546</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>188</v>
+        <v>542</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>189</v>
+        <v>547</v>
       </c>
       <c r="F98" s="6">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G98" s="7"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>344</v>
+        <v>489</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>345</v>
+        <v>490</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>346</v>
+        <v>491</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>347</v>
+        <v>492</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>348</v>
+        <v>493</v>
       </c>
       <c r="F99" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G99" s="7"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>436</v>
+        <v>522</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>437</v>
+        <v>523</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>439</v>
+        <v>524</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>572</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>440</v>
+        <v>525</v>
       </c>
       <c r="F100" s="6">
         <v>1</v>
       </c>
       <c r="G100" s="7"/>
+      <c r="H100" s="17" t="s">
+        <v>591</v>
+      </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A101" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="E101" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="F101" s="6">
+      <c r="A101" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="F101" s="10">
         <v>1</v>
       </c>
-      <c r="G101" s="7"/>
+      <c r="G101" s="11" t="s">
+        <v>578</v>
+      </c>
+      <c r="H101" s="12" t="s">
+        <v>591</v>
+      </c>
+      <c r="I101" s="12" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>317</v>
+        <v>198</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>317</v>
+        <v>199</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>575</v>
+        <v>200</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>319</v>
+        <v>202</v>
       </c>
       <c r="F102" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G102" s="7"/>
-      <c r="H102" s="17" t="s">
-        <v>591</v>
-      </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>320</v>
+        <v>203</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>321</v>
+        <v>204</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>322</v>
+        <v>205</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>323</v>
+        <v>206</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>324</v>
+        <v>207</v>
       </c>
       <c r="F103" s="6">
         <v>2</v>
@@ -4571,135 +4555,127 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>354</v>
+        <v>561</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>355</v>
+        <v>562</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>356</v>
+        <v>563</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>357</v>
+        <v>564</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>358</v>
+        <v>565</v>
       </c>
       <c r="F104" s="6">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="G104" s="7"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>208</v>
+        <v>566</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>209</v>
+        <v>567</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>210</v>
+        <v>568</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>211</v>
+        <v>564</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>212</v>
+        <v>569</v>
       </c>
       <c r="F105" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G105" s="7"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>138</v>
+        <v>190</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>139</v>
+        <v>190</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>140</v>
+        <v>191</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>141</v>
+        <v>190</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>142</v>
+        <v>192</v>
       </c>
       <c r="F106" s="6">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="G106" s="7"/>
+      <c r="I106" t="s">
+        <v>594</v>
+      </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>217</v>
+        <v>181</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>218</v>
+        <v>181</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>571</v>
+        <v>182</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>220</v>
+        <v>184</v>
       </c>
       <c r="F107" s="6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G107" s="7"/>
-      <c r="H107" s="17" t="s">
-        <v>591</v>
-      </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A108" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="B108" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="C108" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>580</v>
-      </c>
-      <c r="E108" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="F108" s="10">
-        <v>1</v>
-      </c>
-      <c r="G108" s="11" t="s">
-        <v>578</v>
-      </c>
-      <c r="H108" s="12" t="s">
-        <v>591</v>
-      </c>
-      <c r="I108" s="12" t="s">
-        <v>593</v>
-      </c>
+      <c r="A108" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="F108" s="6">
+        <v>2</v>
+      </c>
+      <c r="G108" s="7"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>412</v>
+        <v>193</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>413</v>
+        <v>194</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>414</v>
+        <v>195</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>415</v>
+        <v>196</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>416</v>
+        <v>197</v>
       </c>
       <c r="F109" s="6">
         <v>1</v>
@@ -4708,373 +4684,397 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>263</v>
+        <v>221</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>282</v>
+        <v>222</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>283</v>
+        <v>223</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>284</v>
+        <v>224</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>285</v>
+        <v>225</v>
       </c>
       <c r="F110" s="6">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G110" s="7"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>263</v>
+        <v>226</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>264</v>
+        <v>227</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>265</v>
+        <v>228</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>266</v>
+        <v>229</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>267</v>
+        <v>230</v>
       </c>
       <c r="F111" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G111" s="7"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>384</v>
+        <v>208</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>385</v>
+        <v>209</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>386</v>
+        <v>210</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>387</v>
+        <v>211</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>388</v>
+        <v>212</v>
       </c>
       <c r="F112" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G112" s="7"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>313</v>
+        <v>231</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>313</v>
+        <v>232</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="D113" s="4" t="s">
-        <v>315</v>
+        <v>233</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>234</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>316</v>
+        <v>235</v>
       </c>
       <c r="F113" s="6">
+        <v>1</v>
+      </c>
+      <c r="G113" s="7"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="F114" s="6">
         <v>2</v>
       </c>
-      <c r="G113" s="7"/>
-      <c r="H113" s="17" t="s">
+      <c r="G114" s="7"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A115" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="C115" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="E115" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="F115" s="10">
+        <v>2</v>
+      </c>
+      <c r="G115" s="11" t="s">
+        <v>578</v>
+      </c>
+      <c r="H115" s="12" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A114" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E114" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="F114" s="6">
-        <v>6</v>
-      </c>
-      <c r="G114" s="7"/>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A115" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>576</v>
-      </c>
-      <c r="D115" s="3" t="s">
-        <v>573</v>
-      </c>
-      <c r="E115" s="5">
-        <v>61413002</v>
-      </c>
-      <c r="F115" s="6">
-        <v>17</v>
-      </c>
-      <c r="G115" s="7"/>
-      <c r="H115" t="s">
+      <c r="I115" s="12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A116" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="C116" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="E116" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="F116" s="10">
+        <v>2</v>
+      </c>
+      <c r="G116" s="11" t="s">
+        <v>578</v>
+      </c>
+      <c r="H116" s="12" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A116" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="D116" s="3" t="s">
-        <v>574</v>
-      </c>
-      <c r="E116" s="5">
-        <v>61413003</v>
-      </c>
-      <c r="F116" s="6">
-        <v>17</v>
-      </c>
-      <c r="G116" s="7"/>
-      <c r="H116" t="s">
+      <c r="I116" s="12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A117" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="C117" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="E117" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="F117" s="10">
+        <v>1</v>
+      </c>
+      <c r="G117" s="11" t="s">
+        <v>578</v>
+      </c>
+      <c r="H117" s="12" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A117" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="E117" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="F117" s="6">
-        <v>2</v>
-      </c>
-      <c r="G117" s="7"/>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I117" s="12" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>379</v>
+        <v>217</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>380</v>
+        <v>218</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>382</v>
+        <v>219</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>571</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>383</v>
+        <v>220</v>
       </c>
       <c r="F118" s="6">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="G118" s="7"/>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H118" s="17" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>171</v>
+        <v>412</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>172</v>
+        <v>413</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>173</v>
+        <v>414</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>174</v>
+        <v>415</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>175</v>
+        <v>416</v>
       </c>
       <c r="F119" s="6">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G119" s="7"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>203</v>
+        <v>263</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>204</v>
+        <v>264</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>205</v>
+        <v>265</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>206</v>
+        <v>266</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="F120" s="6">
         <v>2</v>
       </c>
       <c r="G120" s="7"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>111</v>
+        <v>263</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>112</v>
+        <v>282</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>113</v>
+        <v>283</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>114</v>
+        <v>284</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>115</v>
+        <v>285</v>
       </c>
       <c r="F121" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G121" s="7"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>116</v>
+        <v>398</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>117</v>
+        <v>399</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>118</v>
+        <v>400</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>114</v>
+        <v>401</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>119</v>
+        <v>402</v>
       </c>
       <c r="F122" s="6">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="G122" s="7"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>494</v>
+        <v>320</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>495</v>
+        <v>321</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>496</v>
+        <v>322</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>497</v>
+        <v>323</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>498</v>
+        <v>324</v>
       </c>
       <c r="F123" s="6">
         <v>2</v>
       </c>
       <c r="G123" s="7"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>403</v>
+        <v>313</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>403</v>
+        <v>313</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>405</v>
+        <v>314</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>315</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>406</v>
+        <v>316</v>
       </c>
       <c r="F124" s="6">
         <v>2</v>
       </c>
       <c r="G124" s="7"/>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H124" s="17" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>272</v>
+        <v>317</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>273</v>
+        <v>317</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>275</v>
+        <v>318</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>575</v>
       </c>
       <c r="E125" s="5" t="s">
-        <v>276</v>
+        <v>319</v>
       </c>
       <c r="F125" s="6">
+        <v>3</v>
+      </c>
+      <c r="G125" s="7"/>
+      <c r="H125" s="17" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A126" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B126" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G125" s="7"/>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A126" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="E126" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="F126" s="6">
-        <v>1</v>
-      </c>
-      <c r="G126" s="7"/>
+      <c r="C126" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E126" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F126" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G126" s="15"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:H127">
-    <sortCondition ref="D1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J126">
+    <sortCondition ref="E16"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="8" orientation="landscape" blackAndWhite="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added 18990006 to database
</commit_message>
<xml_diff>
--- a/Footprints/C655_Main_Board_Footprints_200210.xlsx
+++ b/Footprints/C655_Main_Board_Footprints_200210.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erlendm\OneDrive - Tomra\Arbeidsfiler\GitHub\Tomra_Altium_Library_GitHub\Footprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{E00FA851-567C-42B9-8CDF-AFA10DCA6149}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5EA57834-1900-4DF0-9853-02A664303135}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{E00FA851-567C-42B9-8CDF-AFA10DCA6149}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{634DFDC8-4964-4EA5-86AA-31EC3A76965B}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2267,7 +2267,7 @@
   <dimension ref="A1:J126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E1:E1048576"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2275,7 +2275,8 @@
     <col min="1" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="25.85546875" customWidth="1"/>
     <col min="4" max="4" width="34.42578125" customWidth="1"/>
-    <col min="5" max="6" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
     <col min="10" max="10" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>